<commit_message>
updated template signal and pinout sheets
</commit_message>
<xml_diff>
--- a/Project Template/2 Architecture/Product Architecture Template.xlsx
+++ b/Project Template/2 Architecture/Product Architecture Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="3780" windowWidth="24480" windowHeight="13860" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Major Signals List" sheetId="1" r:id="rId1"/>
-    <sheet name="Pinouts" sheetId="2" r:id="rId2"/>
+    <sheet name="Interface Pinouts" sheetId="2" r:id="rId2"/>
     <sheet name="Current Budget" sheetId="3" r:id="rId3"/>
     <sheet name="Calculations" sheetId="4" r:id="rId4"/>
   </sheets>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t>Project</t>
   </si>
@@ -48,13 +48,7 @@
     <t>Max frequency</t>
   </si>
   <si>
-    <t>Max length</t>
-  </si>
-  <si>
     <t>Copper Weight</t>
-  </si>
-  <si>
-    <t>Min Trace Width</t>
   </si>
   <si>
     <t>Pin Number</t>
@@ -114,14 +108,17 @@
     <t>Max Voltage</t>
   </si>
   <si>
-    <t>COMPONENT NAME</t>
+    <t>Connected Signal</t>
+  </si>
+  <si>
+    <t>INTERFACE NAME</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -146,6 +143,12 @@
       <u/>
       <sz val="10"/>
       <color theme="11"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -187,7 +190,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -212,6 +215,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -564,7 +568,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:G8"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -608,7 +612,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>5</v>
@@ -620,14 +624,10 @@
         <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -642,53 +642,57 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="10"/>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="10"/>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1">
+    <row r="4" spans="1:3" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="10"/>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1">
+    <row r="6" spans="1:3" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="3"/>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1">
+    <row r="7" spans="1:3" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -758,22 +762,22 @@
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1">
       <c r="B6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>15</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B7" s="7">
         <v>1</v>
@@ -788,7 +792,7 @@
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B8" s="7">
         <v>0.05</v>
@@ -803,7 +807,7 @@
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B9" s="7">
         <v>1</v>
@@ -818,7 +822,7 @@
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B10" s="7">
         <v>0.1</v>
@@ -833,7 +837,7 @@
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B11" s="7">
         <v>0.1</v>
@@ -848,7 +852,7 @@
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B12" s="7">
         <v>0.1</v>
@@ -863,7 +867,7 @@
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B13" s="7">
         <v>0</v>
@@ -878,7 +882,7 @@
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B14" s="7">
         <v>1</v>
@@ -893,7 +897,7 @@
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B15" s="7">
         <v>1</v>
@@ -908,7 +912,7 @@
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B16" s="7">
         <v>1</v>
@@ -923,7 +927,7 @@
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B17" s="7">
         <v>1</v>
@@ -938,7 +942,7 @@
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -5868,7 +5872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>